<commit_message>
Waveform diagrams added. New operating modes!
</commit_message>
<xml_diff>
--- a/doc/data packet structure.xlsx
+++ b/doc/data packet structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkiselev\Documents\dev\avr-python-control\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E49A21-3131-4324-9174-6109291950EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2068027-54B1-4BD0-B7FA-FAE32B6502CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{48FB7E95-C391-4754-94A5-34D8116DC883}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <r>
       <t xml:space="preserve">uint8 </t>
@@ -846,6 +846,42 @@
       </rPr>
       <t>inject_delay_cts</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">uint8      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'E'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">uint16                       </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>exposure_time</t>
+    </r>
+  </si>
+  <si>
+    <t>struct Timer1 T1</t>
   </si>
 </sst>
 </file>
@@ -1130,21 +1166,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1229,6 +1250,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1543,10 +1579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C99CE55-3FCF-4F7D-B7A8-CFA50EF16D86}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="C9" sqref="C9:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1558,253 +1594,273 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="31" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K2" s="31"/>
+      <c r="K2" s="26"/>
     </row>
     <row r="3" spans="1:12" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="28"/>
-      <c r="B3" s="26" t="s">
+      <c r="A3" s="23"/>
+      <c r="B3" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="12" t="s">
+      <c r="C3" s="24"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="22" t="s">
+      <c r="J4" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="33"/>
-      <c r="L4" s="27" t="s">
+      <c r="K4" s="28"/>
+      <c r="L4" s="22" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="13" t="s">
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="13" t="s">
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="14" t="s">
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="9" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3" t="s">
+      <c r="D8" s="33"/>
+      <c r="E8" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3" t="s">
+      <c r="F8" s="33"/>
+      <c r="G8" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3" t="s">
+      <c r="H8" s="33"/>
+      <c r="I8" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="15" t="s">
+      <c r="J8" s="34"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="16" t="s">
-        <v>25</v>
+      <c r="B9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="36"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="36"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="17" t="s">
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="1">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
         <v>0</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C12" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D12" s="1">
         <v>2</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E12" s="1">
         <v>3</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F12" s="1">
         <v>4</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G12" s="1">
         <v>5</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H12" s="1">
         <v>6</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I12" s="1">
         <v>7</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J12" s="1">
         <v>8</v>
       </c>
-      <c r="K11" s="35"/>
+      <c r="K12" s="30"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="I8:J8"/>
+    <mergeCell ref="C10:D10"/>
     <mergeCell ref="C9:D9"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Note about sending DONE when completed
</commit_message>
<xml_diff>
--- a/doc/data packet structure.xlsx
+++ b/doc/data packet structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkiselev\Documents\dev\avr-python-control\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C864DE1A-89E8-49D7-BC2E-179E427047D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77DBA8D-D23F-4366-862D-CE4C743666B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{48FB7E95-C391-4754-94A5-34D8116DC883}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
   <si>
     <r>
       <t xml:space="preserve">uint8       </t>
@@ -1128,6 +1128,32 @@
         <scheme val="minor"/>
       </rPr>
       <t>T</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Once the data acquisition is completed, the reply is </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DONE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\n</t>
     </r>
   </si>
 </sst>
@@ -1592,9 +1618,18 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1602,15 +1637,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1935,10 +1961,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2074,10 +2100,10 @@
       <c r="B7" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="48"/>
+      <c r="D7" s="51"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
@@ -2128,14 +2154,14 @@
       <c r="B9" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49" t="s">
+      <c r="D9" s="48"/>
+      <c r="E9" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="46"/>
+      <c r="F9" s="49"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
@@ -2155,22 +2181,22 @@
       <c r="B10" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49" t="s">
+      <c r="D10" s="48"/>
+      <c r="E10" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49" t="s">
+      <c r="F10" s="48"/>
+      <c r="G10" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="49"/>
-      <c r="I10" s="50" t="s">
+      <c r="H10" s="48"/>
+      <c r="I10" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="51"/>
+      <c r="J10" s="46"/>
       <c r="K10" s="19"/>
       <c r="L10" s="6" t="s">
         <v>59</v>
@@ -2186,10 +2212,10 @@
       <c r="B11" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="46"/>
+      <c r="D11" s="49"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
@@ -2326,6 +2352,11 @@
     <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Writing a register does not result in reply
</commit_message>
<xml_diff>
--- a/doc/data packet structure.xlsx
+++ b/doc/data packet structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkiselev\Documents\dev\avr-python-control\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77DBA8D-D23F-4366-862D-CE4C743666B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297DD66F-81A7-4CA3-A7EA-DE2E9F2FFA69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{48FB7E95-C391-4754-94A5-34D8116DC883}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="61">
   <si>
     <r>
       <t xml:space="preserve">uint8       </t>
@@ -1963,8 +1963,8 @@
   </sheetPr>
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2092,9 +2092,7 @@
       <c r="M6" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="N6" s="35" t="s">
-        <v>48</v>
-      </c>
+      <c r="N6" s="35"/>
     </row>
     <row r="7" spans="1:14" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="39" t="s">

</xml_diff>

<commit_message>
Implemented rudimentary continuous acquisition
</commit_message>
<xml_diff>
--- a/doc/data packet structure.xlsx
+++ b/doc/data packet structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkiselev\Documents\dev\sync_device\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769CC38F-980E-4A5C-A9E0-5D33F7764D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C90E2D1-EAB5-41B5-9FA6-F7E6AC009236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{48FB7E95-C391-4754-94A5-34D8116DC883}"/>
   </bookViews>
@@ -752,6 +752,22 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">uint8       </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lasers</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">uint8        </t>
     </r>
     <r>
@@ -759,7 +775,6 @@
         <b/>
         <i/>
         <sz val="11"/>
-        <color theme="0" tint="-0.249977111117893"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -775,7 +790,6 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="0" tint="-0.249977111117893"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -791,7 +805,6 @@
       <rPr>
         <u/>
         <sz val="11"/>
-        <color theme="0" tint="-0.249977111117893"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -801,28 +814,11 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="0" tint="-0.249977111117893"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>ontinuous imaging</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">uint8       </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>lasers</t>
     </r>
   </si>
 </sst>
@@ -889,7 +885,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -898,7 +893,6 @@
       <b/>
       <i/>
       <sz val="11"/>
-      <color theme="0" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -906,7 +900,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="0" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -914,7 +907,6 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color theme="0" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -922,7 +914,6 @@
     <font>
       <i/>
       <sz val="11"/>
-      <color theme="0" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1255,6 +1246,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1264,7 +1262,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1284,12 +1281,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1614,7 +1605,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1680,10 +1671,10 @@
       <c r="B5" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="35" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="3"/>
@@ -1702,7 +1693,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>7</v>
@@ -1724,12 +1715,12 @@
       <c r="B7" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="35"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="38"/>
       <c r="G7" s="13"/>
       <c r="H7" s="18" t="s">
         <v>45</v>
@@ -1745,12 +1736,12 @@
       <c r="B8" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="35"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="38"/>
       <c r="G8" s="13"/>
       <c r="H8" s="18" t="s">
         <v>46</v>
@@ -1763,23 +1754,23 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="38" t="s">
+      <c r="B9" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="42" t="s">
+      <c r="C9" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="42" t="s">
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="43" t="s">
+      <c r="J9" s="45" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1787,12 +1778,12 @@
       <c r="B10" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="35"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="38"/>
       <c r="G10" s="13"/>
       <c r="H10" s="18" t="s">
         <v>50</v>
@@ -1808,12 +1799,12 @@
       <c r="B11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="35"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="38"/>
       <c r="G11" s="13"/>
       <c r="H11" s="18" t="s">
         <v>52</v>
@@ -1829,12 +1820,12 @@
       <c r="B12" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="35"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="38"/>
       <c r="G12" s="13"/>
       <c r="H12" s="18" t="s">
         <v>26</v>
@@ -1913,7 +1904,7 @@
       <c r="B19" t="s">
         <v>23</v>
       </c>
-      <c r="N19" s="36" t="s">
+      <c r="N19" s="33" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Documentation: overview of how system works and detailed description of stroboscopic imaging mode
</commit_message>
<xml_diff>
--- a/doc/data packet structure.xlsx
+++ b/doc/data packet structure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkiselev\Documents\dev\sync_device\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C90E2D1-EAB5-41B5-9FA6-F7E6AC009236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D495477-F2AA-40EF-B832-40D65B998326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{48FB7E95-C391-4754-94A5-34D8116DC883}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
   <si>
     <r>
       <t xml:space="preserve">uint8       </t>
@@ -312,9 +312,6 @@
     </r>
   </si>
   <si>
-    <t>i</t>
-  </si>
-  <si>
     <t>Reply</t>
   </si>
   <si>
@@ -376,7 +373,7 @@
   </si>
   <si>
     <r>
-      <t>Stop (</t>
+      <t xml:space="preserve">Start </t>
     </r>
     <r>
       <rPr>
@@ -387,6 +384,415 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>troboscopic imaging</t>
+    </r>
+  </si>
+  <si>
+    <t>Each data packet is always 5 byte long. If shorter than that, pad it with zeros.</t>
+  </si>
+  <si>
+    <t>Wrong formatted packets are silently ignored (wrong command or too short data packet).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If a command has wrong argument values, the reply is </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ERR\n</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">uint8        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'I'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">uint8        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'A'</t>
+    </r>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Modes: C - continuous, S - stroboscopic (includes ALEX and timelapse)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">uint32                                 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n_frames</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">On startup, the system prints </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Synchronization device is ready. Firmware version: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;x.y.z&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">uint32                   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>acq_period_us</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Set </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cquisition period between frames/bursts</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Set laser </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>xposure time</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">uint32                       </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>exp_time_us</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">uint8        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'D'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">uint32                                </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>shutter_delay_us</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Set shutter </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>elay</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">uint32                                </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cam_readout_us</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Set camera readout </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nterval</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">uint8       </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lasers</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">uint8        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'C'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">uint32                                </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n_frames</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Start </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ontinuous imaging</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Stop acquisition (</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Q</t>
     </r>
     <r>
@@ -398,427 +804,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>uit)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Start </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>S</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>troboscopic imaging</t>
-    </r>
-  </si>
-  <si>
-    <t>Each data packet is always 5 byte long. If shorter than that, pad it with zeros.</t>
-  </si>
-  <si>
-    <t>Wrong formatted packets are silently ignored (wrong command or too short data packet).</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">If a command has wrong argument values, the reply is </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ERR\n</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">uint8        </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'I'</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">uint8        </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'A'</t>
-    </r>
-  </si>
-  <si>
-    <t>Mode</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Modes: C - continuous, S - stroboscopic (includes ALEX and timelapse)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">uint32                                 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>n_frames</t>
-    </r>
-  </si>
-  <si>
-    <t>ToDo</t>
-  </si>
-  <si>
-    <t>ALEX on/off</t>
-  </si>
-  <si>
-    <t>Set spectral channels</t>
-  </si>
-  <si>
-    <t>Start continuous</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">On startup, the system prints </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Synchronization device is ready. Firmware version: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;x.y.z&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>\n</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">uint32                   </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>acq_period_us</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Set </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>A</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cquisition period between frames/bursts</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Set laser </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>xposure time</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">uint32                       </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>exp_time_us</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">uint8        </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'D'</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">uint32                                </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>shutter_delay_us</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Set shutter </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>elay</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">uint32                                </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cam_readout_us</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Set camera readout </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>I</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>nterval</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">uint8       </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>lasers</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">uint8        </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'C'</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">uint32                                </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>n_frames</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Start </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ontinuous imaging</t>
     </r>
   </si>
 </sst>
@@ -826,7 +811,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -918,6 +903,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1154,7 +1146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1253,25 +1245,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1282,6 +1256,30 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1605,7 +1603,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1624,6 +1622,21 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="46">
+        <v>0</v>
+      </c>
+      <c r="C2" s="46">
+        <v>1</v>
+      </c>
+      <c r="D2" s="46">
+        <v>2</v>
+      </c>
+      <c r="E2" s="46">
+        <v>3</v>
+      </c>
+      <c r="F2" s="46">
+        <v>4</v>
+      </c>
       <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1640,202 +1653,202 @@
         <v>12</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="16"/>
+      <c r="B4" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="4"/>
       <c r="G4" s="13"/>
       <c r="H4" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" s="20" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="21" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="35" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="45"/>
       <c r="G5" s="13"/>
       <c r="H5" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="21"/>
+      <c r="J5" s="21" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="45"/>
       <c r="G6" s="13"/>
       <c r="H6" s="18" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="I6" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="I7" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="J7" s="21" t="s">
-        <v>20</v>
+      <c r="J7" s="39" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="38"/>
+        <v>42</v>
+      </c>
+      <c r="C8" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="45"/>
       <c r="G8" s="13"/>
       <c r="H8" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="I8" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="J8" s="21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="44" t="s">
-        <v>56</v>
-      </c>
-      <c r="I9" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="J9" s="45" t="s">
-        <v>20</v>
+      <c r="I9" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="38"/>
+        <v>11</v>
+      </c>
+      <c r="C10" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="45"/>
       <c r="G10" s="13"/>
       <c r="H10" s="18" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="38"/>
+      <c r="B11" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="16"/>
       <c r="G11" s="13"/>
       <c r="H11" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="I11" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="J11" s="21" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="I11" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="38"/>
+        <v>1</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4"/>
       <c r="G12" s="13"/>
       <c r="H12" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="J12" s="21" t="s">
-        <v>20</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="I12" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="21"/>
     </row>
     <row r="13" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="26" t="s">
@@ -1847,32 +1860,30 @@
       <c r="F13" s="6"/>
       <c r="G13" s="13"/>
       <c r="H13" s="18" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="I13" s="18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J13" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="1">
+      <c r="A14" s="22"/>
+      <c r="B14" s="46">
         <v>0</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="47">
         <v>1</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="46">
         <v>2</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="46">
         <v>3</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="46">
         <v>4</v>
       </c>
       <c r="G14" s="14"/>
@@ -1892,76 +1903,63 @@
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>23</v>
-      </c>
-      <c r="N19" s="33" t="s">
-        <v>39</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="N19" s="33"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>37</v>
-      </c>
-      <c r="N20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="N21" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B23" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>28</v>
-      </c>
-      <c r="N25" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C5:F5"/>
     <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C12:F12"/>
     <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="110" fitToWidth="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added "M" command to manually open laser shutters
</commit_message>
<xml_diff>
--- a/doc/data packet structure.xlsx
+++ b/doc/data packet structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkiselev\Documents\dev\sync_device\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D495477-F2AA-40EF-B832-40D65B998326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECB9A70-B195-4AAB-B538-2A64807A377B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{48FB7E95-C391-4754-94A5-34D8116DC883}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{48FB7E95-C391-4754-94A5-34D8116DC883}"/>
   </bookViews>
   <sheets>
     <sheet name="Data packet format" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
   <si>
     <r>
       <t xml:space="preserve">uint8       </t>
@@ -107,9 +107,6 @@
     </r>
   </si>
   <si>
-    <t>Data packet format</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">uint8     </t>
     </r>
@@ -405,6 +402,436 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">uint8        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'I'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">uint8        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'A'</t>
+    </r>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Modes: C - continuous, S - stroboscopic (includes ALEX and timelapse)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">uint32                                 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n_frames</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">On startup, the system prints </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Synchronization device is ready. Firmware version: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;x.y.z&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">uint32                   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>acq_period_us</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Set </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cquisition period between frames/bursts</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Set laser </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>xposure time</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">uint32                       </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>exp_time_us</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">uint8        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'D'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">uint32                                </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>shutter_delay_us</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Set shutter </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>elay</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">uint32                                </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cam_readout_us</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Set camera readout </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nterval</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">uint8       </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lasers</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">uint8        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'C'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">uint32                                </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n_frames</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Start </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ontinuous imaging</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Stop acquisition (</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Q</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>uit)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">uint8        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'M'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>anually open laser shutters</t>
+    </r>
+  </si>
+  <si>
+    <t>Sync device data packet format</t>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">If a command has wrong argument values, the reply is </t>
     </r>
     <r>
@@ -418,392 +845,15 @@
       </rPr>
       <t>ERR\n</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">uint8        </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'I'</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">uint8        </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'A'</t>
-    </r>
-  </si>
-  <si>
-    <t>Mode</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Modes: C - continuous, S - stroboscopic (includes ALEX and timelapse)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">uint32                                 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>n_frames</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">On startup, the system prints </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Synchronization device is ready. Firmware version: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;x.y.z&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>\n</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">uint32                   </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>acq_period_us</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Set </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>A</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cquisition period between frames/bursts</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Set laser </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>xposure time</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">uint32                       </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>exp_time_us</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">uint8        </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'D'</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">uint32                                </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>shutter_delay_us</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Set shutter </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>elay</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">uint32                                </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cam_readout_us</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Set camera readout </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>I</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>nterval</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">uint8       </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>lasers</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">uint8        </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'C'</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">uint32                                </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>n_frames</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Start </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ontinuous imaging</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Stop acquisition (</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Q</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>uit)</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (NOT IMPLEMENTED)</t>
     </r>
   </si>
 </sst>
@@ -936,7 +986,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1037,43 +1087,9 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <left/>
+      <right/>
       <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -1087,17 +1103,6 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1124,29 +1129,27 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1211,25 +1214,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1239,15 +1233,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1257,21 +1242,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1280,6 +1250,36 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1600,10 +1600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6FE895D-0C3B-46E0-B798-2A07ED6015B0}">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1618,23 +1618,23 @@
   <sheetData>
     <row r="1" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B1" s="23" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="46">
+      <c r="B2" s="35">
         <v>0</v>
       </c>
-      <c r="C2" s="46">
+      <c r="C2" s="35">
         <v>1</v>
       </c>
-      <c r="D2" s="46">
+      <c r="D2" s="35">
         <v>2</v>
       </c>
-      <c r="E2" s="46">
+      <c r="E2" s="35">
         <v>3</v>
       </c>
-      <c r="F2" s="46">
+      <c r="F2" s="35">
         <v>4</v>
       </c>
       <c r="G2" s="11"/>
@@ -1650,306 +1650,325 @@
       <c r="F3" s="10"/>
       <c r="G3" s="12"/>
       <c r="H3" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="28" t="s">
-        <v>7</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>6</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="4"/>
       <c r="G4" s="13"/>
       <c r="H4" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I4" s="18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J4" s="21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="43" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="45"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="42"/>
       <c r="G5" s="13"/>
       <c r="H5" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" s="21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="45"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="42"/>
       <c r="G6" s="13"/>
       <c r="H6" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="J7" s="33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" s="21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="I7" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="J7" s="39" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="45"/>
+      <c r="C8" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="42"/>
       <c r="G8" s="13"/>
       <c r="H8" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J8" s="21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="45"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="42"/>
       <c r="G9" s="13"/>
       <c r="H9" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J9" s="21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="45"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="42"/>
       <c r="G10" s="13"/>
       <c r="H10" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="44"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
       <c r="F11" s="16"/>
       <c r="G11" s="13"/>
       <c r="H11" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="J11" s="20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="35" t="s">
-        <v>6</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="28"/>
+      <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="4"/>
       <c r="G12" s="13"/>
       <c r="H12" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="J12" s="21"/>
-    </row>
-    <row r="13" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="6"/>
+        <v>49</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="4"/>
       <c r="G13" s="13"/>
       <c r="H13" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="I13" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="J13" s="21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
-      <c r="B14" s="46">
+        <v>13</v>
+      </c>
+      <c r="I13" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="21"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="22"/>
+      <c r="B15" s="35">
         <v>0</v>
       </c>
-      <c r="C14" s="47">
+      <c r="C15" s="36">
         <v>1</v>
       </c>
-      <c r="D14" s="46">
+      <c r="D15" s="35">
         <v>2</v>
       </c>
-      <c r="E14" s="46">
+      <c r="E15" s="35">
         <v>3</v>
       </c>
-      <c r="F14" s="46">
+      <c r="F15" s="35">
         <v>4</v>
       </c>
-      <c r="G14" s="14"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
       <c r="G15" s="14"/>
     </row>
-    <row r="16" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="2" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="N19" s="33"/>
+        <v>20</v>
+      </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B22" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B23" s="19" t="s">
-        <v>25</v>
+        <v>21</v>
+      </c>
+      <c r="N20" s="30"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>37</v>
+      <c r="B24" s="19" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>23</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1961,7 +1980,7 @@
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="C8:F8"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="110" fitToWidth="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>